<commit_message>
Revert "Merge branch 'main' of https://github.com/pradeepkumar24rk/JavaProgramming"
This reverts commit 43011fffee6848972b3dadc8611571a6d220f1d4, reversing
changes made to d601bfe5d24af9eac1d4b00427e025f627003255.
</commit_message>
<xml_diff>
--- a/topics to study.xlsx
+++ b/topics to study.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hai\Music\Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A29E7B9-E664-4E85-B1ED-D23CF51B9600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEF34BF-436F-455B-A49C-E08D7454A26D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1492,27 +1492,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -1520,21 +1508,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1558,13 +1537,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1584,9 +1556,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1624,7 +1596,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1730,7 +1702,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1872,7 +1844,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1880,35 +1852,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
-  <dimension ref="A1:D481"/>
+  <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="28.5" customWidth="1"/>
     <col min="2" max="2" width="123" customWidth="1"/>
     <col min="3" max="3" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24.6">
+    <row r="1" spans="1:3" ht="25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:3">
       <c r="B2" s="10" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:3">
       <c r="B3" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="21">
+    <row r="4" spans="1:3" ht="21">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1919,46 +1891,45 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="C5" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="13"/>
-    </row>
-    <row r="6" spans="1:4" ht="21">
+    <row r="5" spans="1:3">
+      <c r="C5" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="21">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="21">
+      <c r="C6" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="21">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="21">
+      <c r="C7" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="21">
       <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="21">
+      <c r="C8" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="21">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
@@ -1969,7 +1940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="21">
+    <row r="10" spans="1:3" ht="21">
       <c r="A10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1980,7 +1951,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="21">
+    <row r="11" spans="1:3" ht="21">
       <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
@@ -1991,7 +1962,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="21">
+    <row r="12" spans="1:3" ht="21">
       <c r="A12" s="5" t="s">
         <v>5</v>
       </c>
@@ -2002,7 +1973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="21">
+    <row r="13" spans="1:3" ht="21">
       <c r="A13" s="5" t="s">
         <v>5</v>
       </c>
@@ -2013,7 +1984,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="21">
+    <row r="14" spans="1:3" ht="21">
       <c r="A14" s="5" t="s">
         <v>5</v>
       </c>
@@ -2024,7 +1995,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="21">
+    <row r="15" spans="1:3" ht="21">
       <c r="A15" s="5" t="s">
         <v>5</v>
       </c>
@@ -2035,7 +2006,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="21">
+    <row r="16" spans="1:3" ht="21">
       <c r="A16" s="5" t="s">
         <v>5</v>
       </c>
@@ -7409,6 +7380,5 @@
     <hyperlink ref="B2" r:id="rId446" xr:uid="{E07D4FE5-46C7-AC4D-9E01-2300AA43B58A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId447"/>
 </worksheet>
 </file>
</xml_diff>